<commit_message>
Se termina desarrollo del a issue
</commit_message>
<xml_diff>
--- a/static/templates/ListadoAdmitidos.xlsx
+++ b/static/templates/ListadoAdmitidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josemasster\go\src\github.com\udistrital\sga_admisiones_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE789DC2-A2E9-4DE2-A3F3-3F6B6E7D6522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BAA085-7617-4289-8BCB-FE5C74050129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15990" xr2:uid="{69B13D3E-9994-4F5C-8636-779CE2B5E8CC}"/>
   </bookViews>
@@ -150,26 +150,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,119 +563,121 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="1" max="6" width="11.5546875" style="7"/>
+    <col min="7" max="7" width="14.88671875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>